<commit_message>
Created First Version of PValue Order Management
</commit_message>
<xml_diff>
--- a/dhan_excel/PValue_Pulse.xlsx
+++ b/dhan_excel/PValue_Pulse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Harvest FinCrop\Algo Trading\dhan_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\SucessfulAlgoTrading\dhan_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F96F33E-750D-4150-81AB-517CBD9F9DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11130DFF-D6BE-4D57-81DB-44EC2C39467C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3F6F1494-9B09-4F57-8AEB-2BA84EF373A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3F6F1494-9B09-4F57-8AEB-2BA84EF373A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Trade" sheetId="1" r:id="rId1"/>
@@ -113,17 +113,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
       <xlwcv:version setVersion="1"/>
     </ext>
@@ -5242,9 +5231,6 @@
     <t>NON SLICE ORDERT QTY</t>
   </si>
   <si>
-    <t>STOP</t>
-  </si>
-  <si>
     <t>NIFTY PE</t>
   </si>
   <si>
@@ -5254,7 +5240,10 @@
     <t>STATUS</t>
   </si>
   <si>
-    <t>OPEN</t>
+    <t>TRADE</t>
+  </si>
+  <si>
+    <t>START</t>
   </si>
 </sst>
 </file>
@@ -5262,10 +5251,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="0.00000%"/>
-    <numFmt numFmtId="166" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="0.00000%"/>
+    <numFmt numFmtId="167" formatCode="&quot;₹&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -5489,7 +5478,7 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5498,7 +5487,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -5527,13 +5516,24 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5544,7 +5544,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -5555,17 +5555,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5710,9 +5699,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5750,7 +5739,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5856,7 +5845,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5998,7 +5987,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6009,8 +5998,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AL37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -6040,27 +6029,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="E1" s="51" t="str">
+      <c r="B1" s="57"/>
+      <c r="E1" s="58" t="str">
         <f>B24</f>
         <v>PE</v>
       </c>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51" t="str">
+      <c r="F1" s="58"/>
+      <c r="G1" s="58" t="str">
         <f>SIDE</f>
         <v>OTM</v>
       </c>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="52">
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="59">
         <f>Charges!H1</f>
         <v>-4233.9525139650004</v>
       </c>
-      <c r="K1" s="52"/>
-      <c r="L1" s="53">
+      <c r="K1" s="59"/>
+      <c r="L1" s="60">
         <f>Charges!K1</f>
         <v>22</v>
       </c>
@@ -6073,14 +6062,14 @@
         <f>INDEX_NAME</f>
         <v>NIFTY PE</v>
       </c>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="53"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="60"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -7945,18 +7934,18 @@
       <c r="G31" s="8"/>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="D32" s="49" t="str">
+      <c r="D32" s="56" t="str">
         <f>IF(AND(LIMITMODE,COUNT(I6:I16)=0,COUNT(J6:J16)&lt;&gt;0),"PROVIDE LIMIT PRICE","")</f>
         <v/>
       </c>
-      <c r="E32" s="49"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="49"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="49"/>
-      <c r="K32" s="49"/>
-      <c r="L32" s="49"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
+      <c r="J32" s="56"/>
+      <c r="K32" s="56"/>
+      <c r="L32" s="56"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
@@ -7965,15 +7954,15 @@
       <c r="B33" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="49"/>
-      <c r="J33" s="49"/>
-      <c r="K33" s="49"/>
-      <c r="L33" s="49"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="56"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="56"/>
+      <c r="L33" s="56"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E34" s="8"/>
@@ -8018,7 +8007,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="5">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B29" xr:uid="{A1FEE6D5-54C4-461C-B04B-7F0563CB22A3}">
       <formula1>"True, False"</formula1>
     </dataValidation>
@@ -8048,7 +8037,7 @@
   <dimension ref="A1:T45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8075,7 +8064,7 @@
         <v>1600</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
@@ -8109,14 +8098,14 @@
       <c r="A3" s="37" t="s">
         <v>1599</v>
       </c>
-      <c r="B3" s="56">
+      <c r="B3" s="49">
         <f>VLOOKUP(TRADEDSERIES,Trade!F6:G16,2,FALSE)</f>
         <v>60454</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>1595</v>
       </c>
-      <c r="E3" s="60">
+      <c r="E3" s="53">
         <f>SUM(TRADEMGMT!E9:E1048574)</f>
         <v>0</v>
       </c>
@@ -8137,20 +8126,20 @@
       <c r="A4" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="56">
+      <c r="B4" s="49">
         <v>0.05</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>1674</v>
       </c>
-      <c r="E4" s="58">
+      <c r="E4" s="51">
         <f>SUMIF(TRADEMGMT!G9:G1048576,ORDERSTATUS,TRADEMGMT!E9:E1048576)</f>
         <v>0</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>1597</v>
       </c>
-      <c r="H4" s="59">
+      <c r="H4" s="52">
         <f>SUMIF(TRADEMGMT!G9:G1048576,ORDERSTATUS,TRADEMGMT!H9:H1048576)</f>
         <v>0</v>
       </c>
@@ -8160,19 +8149,19 @@
         <v>1601</v>
       </c>
       <c r="B5" s="34">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="D5" t="s">
         <v>1672</v>
       </c>
-      <c r="E5" s="58">
+      <c r="E5" s="51">
         <f>COUNT(TRADEMGMT!D9:D1048574)</f>
         <v>4</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>1670</v>
       </c>
-      <c r="H5" s="59">
+      <c r="H5" s="52">
         <f>BUY_ORDER_COST+(BUY_ORDER_COST*PROFIT_EXIT_ACTUAL_PERCENTAGE)</f>
         <v>0</v>
       </c>
@@ -8187,14 +8176,14 @@
       <c r="D6" s="10" t="s">
         <v>1673</v>
       </c>
-      <c r="E6" s="58">
+      <c r="E6" s="51">
         <f>COUNTIF(TRADEMGMT!G9:G1048576,ORDERSTATUS)</f>
         <v>0</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>1671</v>
       </c>
-      <c r="H6" s="59">
+      <c r="H6" s="52">
         <f>BUY_ORDER_COST-(BUY_ORDER_COST*LOSS_EXIT_ACTUAL_PERCENTAGE)</f>
         <v>0</v>
       </c>
@@ -8203,12 +8192,12 @@
       <c r="A7" s="37" t="s">
         <v>1549</v>
       </c>
-      <c r="B7" s="56">
-        <f>IF(ALLOCATION_PCT&lt;&gt;"",
+      <c r="B7" s="49">
+        <f>IF(LMT_PRICE&lt;&gt;"",
                   IF(LMT_PRICE&lt;&gt;"",ROUNDDOWN((CAPITAL*ALLOCATION_PCT)/(LMT_PRICE*LOT_SIZE),0)*LOTSIZEMULTIPLIER,
                  ROUNDDOWN((CAPITAL*ALLOCATION_PCT)/(LTP*LOT_SIZE),0)*LOTSIZEMULTIPLIER),
 "")</f>
-        <v>7200</v>
+        <v>7350</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
@@ -8228,7 +8217,7 @@
         <v>1800</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>1592</v>
@@ -8263,7 +8252,7 @@
         <v>1680</v>
       </c>
       <c r="B9" s="37">
-        <f>ROUNDUP(B7/B8,0)</f>
+        <f>INT(ORDER_PLACED_QTY/B8)</f>
         <v>4</v>
       </c>
       <c r="D9" s="12">
@@ -8279,9 +8268,9 @@
       <c r="A10" s="37" t="s">
         <v>1681</v>
       </c>
-      <c r="B10" s="56">
-        <f>(B9-1)*B8</f>
-        <v>5400</v>
+      <c r="B10" s="49">
+        <f>B9*B8</f>
+        <v>7200</v>
       </c>
       <c r="D10" s="12">
         <v>102250930610802</v>
@@ -8294,9 +8283,9 @@
       <c r="A11" s="37" t="s">
         <v>1682</v>
       </c>
-      <c r="B11" s="56">
-        <f>B8-((B9*B8)-B7)</f>
-        <v>1800</v>
+      <c r="B11" s="49">
+        <f>MOD(ORDER_PLACED_QTY,B8)</f>
+        <v>150</v>
       </c>
       <c r="D11" s="12">
         <v>42250930656302</v>
@@ -8309,17 +8298,17 @@
       <c r="A12" s="37" t="s">
         <v>1594</v>
       </c>
-      <c r="B12" s="57" t="s">
-        <v>1683</v>
-      </c>
-      <c r="D12" s="61">
+      <c r="B12" s="50" t="s">
+        <v>1686</v>
+      </c>
+      <c r="D12" s="54">
         <v>332250930674802</v>
       </c>
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
       <c r="G12" s="31"/>
       <c r="H12" s="31"/>
-      <c r="J12" s="61">
+      <c r="J12" s="54">
         <v>332250930674802</v>
       </c>
       <c r="K12" s="31"/>
@@ -8330,7 +8319,7 @@
     </row>
     <row r="13" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="B13" s="41" t="s">
         <v>1687</v>
@@ -8363,8 +8352,8 @@
       <c r="A16" s="19" t="s">
         <v>1664</v>
       </c>
-      <c r="B16" s="58">
-        <v>7200</v>
+      <c r="B16" s="51">
+        <v>4566</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -8376,32 +8365,32 @@
       <c r="S16" s="10"/>
     </row>
     <row r="17" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="62" t="s">
+      <c r="A17" s="55" t="s">
         <v>1680</v>
       </c>
-      <c r="B17" s="58">
-        <f>ROUNDUP(B16/B8,0)</f>
-        <v>4</v>
+      <c r="B17" s="51">
+        <f>INT(BUY_QTY/B8)</f>
+        <v>2</v>
       </c>
       <c r="D17" s="12"/>
     </row>
     <row r="18" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="62" t="s">
+      <c r="A18" s="55" t="s">
         <v>1681</v>
       </c>
-      <c r="B18" s="58">
-        <f>(B17-1)*B8</f>
-        <v>5400</v>
+      <c r="B18" s="51">
+        <f>B17*B8</f>
+        <v>3600</v>
       </c>
       <c r="D18" s="12"/>
     </row>
     <row r="19" spans="1:19" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="62" t="s">
+      <c r="A19" s="55" t="s">
         <v>1682</v>
       </c>
-      <c r="B19" s="58">
-        <f>B8-((B17*B8)-B16)</f>
-        <v>1800</v>
+      <c r="B19" s="51">
+        <f>MOD(BUY_QTY,B8)</f>
+        <v>966</v>
       </c>
       <c r="D19" s="12"/>
     </row>
@@ -8409,7 +8398,7 @@
       <c r="A20" s="19" t="s">
         <v>1665</v>
       </c>
-      <c r="B20" s="59">
+      <c r="B20" s="52">
         <f>TRADEMGMT!H3</f>
         <v>0</v>
       </c>
@@ -8420,7 +8409,9 @@
       <c r="M20" s="31"/>
       <c r="N20" s="31"/>
       <c r="O20" s="4"/>
-      <c r="P20" s="31"/>
+      <c r="P20" s="31">
+        <v>10000</v>
+      </c>
       <c r="Q20" s="31"/>
       <c r="R20" s="31"/>
       <c r="S20" s="31"/>
@@ -8429,7 +8420,7 @@
       <c r="A21" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="59">
+      <c r="B21" s="52">
         <f>IF(AVG_BUY_PRICE&lt;&gt;"",(AVG_BUY_PRICE+(AVG_BUY_PRICE*PROFT_EXIT_TRIGGER_PERCENTAGE))-MOD((AVG_BUY_PRICE+(AVG_BUY_PRICE*PROFT_EXIT_TRIGGER_PERCENTAGE)),0.05),"")</f>
         <v>0</v>
       </c>
@@ -8440,7 +8431,9 @@
       <c r="M21" s="31"/>
       <c r="N21" s="31"/>
       <c r="O21" s="4"/>
-      <c r="P21" s="31"/>
+      <c r="P21" s="31">
+        <v>0.5</v>
+      </c>
       <c r="Q21" s="31"/>
       <c r="R21" s="31"/>
       <c r="S21" s="31"/>
@@ -8449,7 +8442,7 @@
       <c r="A22" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="59">
+      <c r="B22" s="52">
         <f>IF(AVG_BUY_PRICE&lt;&gt;"",(AVG_BUY_PRICE-(AVG_BUY_PRICE*LOSS_EXIT_TRIGGER_PERCENTAGE))-MOD((AVG_BUY_PRICE-(AVG_BUY_PRICE*LOSS_EXIT_TRIGGER_PERCENTAGE)),0.05),"")</f>
         <v>0</v>
       </c>
@@ -8461,7 +8454,10 @@
       <c r="M22" s="31"/>
       <c r="N22" s="31"/>
       <c r="O22" s="4"/>
-      <c r="P22" s="31"/>
+      <c r="P22" s="31">
+        <f>P20*P21</f>
+        <v>5000</v>
+      </c>
       <c r="Q22" s="31"/>
       <c r="R22" s="31"/>
       <c r="S22" s="31"/>
@@ -8470,7 +8466,7 @@
       <c r="A23" t="s">
         <v>1666</v>
       </c>
-      <c r="B23" s="59">
+      <c r="B23" s="52">
         <f>IF(AVG_BUY_PRICE&lt;&gt;"",(AVG_BUY_PRICE+(AVG_BUY_PRICE*PROFIT_EXIT_ACTUAL_PERCENTAGE))-MOD((AVG_BUY_PRICE+(AVG_BUY_PRICE*PROFIT_EXIT_ACTUAL_PERCENTAGE)),0.05),"")</f>
         <v>0</v>
       </c>
@@ -8481,7 +8477,9 @@
       <c r="M23" s="31"/>
       <c r="N23" s="31"/>
       <c r="O23" s="4"/>
-      <c r="P23" s="31"/>
+      <c r="P23" s="31">
+        <v>50</v>
+      </c>
       <c r="Q23" s="31"/>
       <c r="R23" s="31"/>
       <c r="S23" s="31"/>
@@ -8490,7 +8488,7 @@
       <c r="A24" t="s">
         <v>1667</v>
       </c>
-      <c r="B24" s="59">
+      <c r="B24" s="52">
         <f>IF(AVG_BUY_PRICE&lt;&gt;"",(AVG_BUY_PRICE-(AVG_BUY_PRICE*LOSS_EXIT_ACTUAL_PERCENTAGE))-MOD((AVG_BUY_PRICE-(AVG_BUY_PRICE*LOSS_EXIT_ACTUAL_PERCENTAGE)),0.05),"")</f>
         <v>0</v>
       </c>
@@ -8498,7 +8496,10 @@
       <c r="K24" s="10"/>
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
-      <c r="P24" s="10"/>
+      <c r="P24" s="10">
+        <f>P22/P23</f>
+        <v>100</v>
+      </c>
       <c r="Q24" s="10"/>
       <c r="R24" s="10"/>
       <c r="S24" s="10"/>
@@ -8507,11 +8508,15 @@
       <c r="A25" s="10" t="s">
         <v>1669</v>
       </c>
-      <c r="B25" s="59" t="e">
+      <c r="B25" s="52" t="e">
         <f>IF(B36&lt;&gt;"",(B36-MOD(B36,0.05)),"")</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I25"/>
+      <c r="P25">
+        <f>ROUNDDOWN(P24/75,0)</f>
+        <v>1</v>
+      </c>
       <c r="R25" s="10"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -8520,6 +8525,10 @@
       </c>
       <c r="B26" s="43"/>
       <c r="I26"/>
+      <c r="P26">
+        <f>P25*75</f>
+        <v>75</v>
+      </c>
       <c r="R26" s="10"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -8528,7 +8537,7 @@
       </c>
       <c r="B27" s="45">
         <f>IF(BUY_QTY&lt;&gt;"",BUY_QTY*BROKERAGE*2,"")</f>
-        <v>288000</v>
+        <v>182640</v>
       </c>
       <c r="I27"/>
       <c r="R27" s="10"/>
@@ -8586,6 +8595,10 @@
         <v>0</v>
       </c>
       <c r="I32"/>
+      <c r="P32" s="10">
+        <f>75*5</f>
+        <v>375</v>
+      </c>
       <c r="R32" s="10"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -8594,7 +8607,7 @@
       </c>
       <c r="B33" s="45">
         <f>IF(BUY_QTY&lt;&gt;"",(B27+B28+B31)*CHARGES_GST,"")</f>
-        <v>51840</v>
+        <v>32875.199999999997</v>
       </c>
       <c r="I33"/>
       <c r="R33" s="10"/>
@@ -8605,7 +8618,7 @@
       </c>
       <c r="B34" s="45">
         <f>IF(BUY_QTY&lt;&gt;"",SUM(B27:B33),"")</f>
-        <v>339840</v>
+        <v>215515.2</v>
       </c>
       <c r="I34"/>
       <c r="R34" s="10"/>
@@ -8646,7 +8659,7 @@
       </c>
       <c r="B40" s="41" t="str">
         <f>IF(AND(INITIATE="TRADE",ORDER_PLACED_QTY&gt;0),IF(LMT_PRICE&lt;&gt;"","LIMIT","MARKET"),"")</f>
-        <v/>
+        <v>LIMIT</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
@@ -8669,21 +8682,22 @@
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="3">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1" xr:uid="{212417BE-54D2-46D7-B79B-198CD27529C3}">
-      <formula1>"NIFTY PE, NIFTY CE, BANKNIFTY PE, BANKNIFTY CE,CRUDEOIL CE, CRUDEOIL PE, CRUDEOILM CE, CRUDEOILM PE"</formula1>
+      <formula1>"NIFTY PE, NIFTY CE, BANKNIFTY PE, BANKNIFTY CE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12" xr:uid="{03C9B054-A939-47CB-97F2-9DCC89D49BFD}">
       <formula1>"TRADE, STOP"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13" xr:uid="{7263FF6E-CFF3-41C8-83D6-667A6690EC8E}">
-      <formula1>"OPEN,INITIATED,INPROGRESS,COMPLETE"</formula1>
+      <formula1>"START,PROCESSING,PROCESS-EXIT-PROFIT,PROCESS-EXIT-LOSS,EXIT-PROFIT,EXIT-LOSS,PROCESS-EXIT-BE,EXIT-BE,COMPLETED"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{996C241C-E408-4845-812B-AAB72B96820F}">
           <x14:formula1>
             <xm:f>Trade!$F$6:$F$16</xm:f>
@@ -35421,17 +35435,17 @@
         <f>B2-B1</f>
         <v>-3300</v>
       </c>
-      <c r="G1" s="55" t="s">
+      <c r="G1" s="62" t="s">
         <v>1577</v>
       </c>
-      <c r="H1" s="54">
+      <c r="H1" s="61">
         <f>E1-E2</f>
         <v>-4233.9525139650004</v>
       </c>
-      <c r="J1" s="55" t="s">
+      <c r="J1" s="62" t="s">
         <v>1579</v>
       </c>
-      <c r="K1" s="54">
+      <c r="K1" s="61">
         <f>COUNT(_xlfn.UNIQUE(A4:A52))</f>
         <v>22</v>
       </c>
@@ -35451,10 +35465,10 @@
         <f>SUM(M4:M52)</f>
         <v>933.95251396500009</v>
       </c>
-      <c r="G2" s="55"/>
-      <c r="H2" s="54"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="54"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="61"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="61"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">

</xml_diff>